<commit_message>
updated how disabled works
</commit_message>
<xml_diff>
--- a/R/datasets/Jeopardy.xlsx
+++ b/R/datasets/Jeopardy.xlsx
@@ -130,7 +130,7 @@
     <t xml:space="preserve">ANSWERS </t>
   </si>
   <si>
-    <t>own businesses, register wealth or property, practice medicine, attend non-Jewish schools</t>
+    <t>Own businesses, register wealth or property, practice medicine, attend non-Jewish schools</t>
   </si>
   <si>
     <t>"death camps” or "death factories"</t>
@@ -160,7 +160,7 @@
     <t>owning land, having national health insurance, getting Law degrees</t>
   </si>
   <si>
-    <t>20% (1 in 5)</t>
+    <t>20% (1 in 5) of people</t>
   </si>
   <si>
     <t>Mercy Death program</t>
@@ -178,7 +178,11 @@
     <t>They viewed them as unworthy of life, and useless people who were a burden upon society.</t>
   </si>
   <si>
-    <t>Americans with Disabilities Act, Section 504, Individuals with Disabilities Education Act, Rehabilitation Act, United Nations Convention on the Rights of Persons with Disabilities</t>
+    <t>Americans with Disabilities Act, 
+Section 504, 
+Individuals with Disabilities Education Act,
+Rehabilitation Act, 
+United Nations Convention on the Rights of Persons with Disabilities</t>
   </si>
   <si>
     <t xml:space="preserve">HEX </t>

</xml_diff>